<commit_message>
new TextEncoder support cryptoHash
</commit_message>
<xml_diff>
--- a/doc/Type2.xlsx
+++ b/doc/Type2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC896C6-F393-4205-AD58-F65BE4FCCFFB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67BCA8A-1D9F-48F0-B05E-DC4DE8D82D08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="17">
   <si>
     <t>_expire</t>
   </si>
@@ -401,7 +401,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +610,9 @@
       <c r="H15" t="s">
         <v>9</v>
       </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
       <c r="L15" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>